<commit_message>
add video-question and variable xlsx files
</commit_message>
<xml_diff>
--- a/test files/test.xlsx
+++ b/test files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12000" tabRatio="500"/>
+    <workbookView windowWidth="27900" windowHeight="12000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Вопросы" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>THEME</t>
   </si>
@@ -35,9 +35,6 @@
     <t>В Древней Руси деньгами служили серебряные бруски. Их называли гривнами. Если вещь стоила меньше, чем весь брусок, то от него отрубали часть. Как называлась отрубленная часть серебряного бруска?</t>
   </si>
   <si>
-    <t>Две дочери, две матери, да бабушка с внучкой. Сколько всех?</t>
-  </si>
-  <si>
     <t>Космос</t>
   </si>
   <si>
@@ -50,10 +47,7 @@
     <t>Почему на Солнце есть пятна?</t>
   </si>
   <si>
-    <t>Какая из планет самая горячая?</t>
-  </si>
-  <si>
-    <t>В честь чего празднуется день космонавтики</t>
+    <t>video.avi</t>
   </si>
   <si>
     <t>Искусство </t>
@@ -71,9 +65,6 @@
     <t>девочка_с_персиками.jpeg</t>
   </si>
   <si>
-    <t>звездная-ночь.jpg</t>
-  </si>
-  <si>
     <t>Математика </t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>Какой угол образуют стрелки часов, показывающие три часа?</t>
   </si>
   <si>
-    <t>Сколько вершин у параллелепипеда?</t>
-  </si>
-  <si>
     <t>Кот в мешке</t>
   </si>
   <si>
@@ -104,10 +92,7 @@
     <t>Между какими двумя одинаковыми буквами можно поставить маленькую лошадь и получить название страны?</t>
   </si>
   <si>
-    <t>Друг зверей и друг детей добрый доктор…</t>
-  </si>
-  <si>
-    <t>Как приезжему отыскать площадь Горького?</t>
+    <t>video.mp4</t>
   </si>
   <si>
     <t>Фильмы</t>
@@ -123,9 +108,6 @@
   </si>
   <si>
     <t>Титаник.jpg</t>
-  </si>
-  <si>
-    <t>Острые-Козырьки.jpg</t>
   </si>
   <si>
     <t>Ми-ля-ми</t>
@@ -224,9 +206,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -246,16 +228,128 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,129 +363,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,61 +388,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,13 +556,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,103 +568,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,11 +582,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,6 +636,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -656,10 +664,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -673,175 +679,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1183,8 +1165,8 @@
   <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="5"/>
@@ -1208,14 +1190,12 @@
         <v>200</v>
       </c>
       <c r="D1" s="2">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="E1" s="2">
         <v>400</v>
       </c>
-      <c r="F1" s="2">
-        <v>500</v>
-      </c>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" s="4" customFormat="1" ht="140" customHeight="1" spans="1:6">
       <c r="A2" s="3" t="s">
@@ -1233,109 +1213,97 @@
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" s="4" customFormat="1" ht="75" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" s="4" customFormat="1" ht="70" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" s="4" customFormat="1" ht="66" customHeight="1" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" s="4" customFormat="1" ht="90" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" s="4" customFormat="1" ht="64" customHeight="1" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1349,8 +1317,8 @@
   <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.4" outlineLevelRow="6" outlineLevelCol="5"/>
@@ -1375,7 +1343,7 @@
         <v>200</v>
       </c>
       <c r="D1" s="2">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="E1" s="2">
         <v>400</v>
@@ -1389,119 +1357,119 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" ht="99" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" ht="49" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" ht="58" customHeight="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" ht="50" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" ht="47" customHeight="1" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>